<commit_message>
add xlsx for wrappers testing
</commit_message>
<xml_diff>
--- a/quickstart/jsonbox_test_api_just_wrapper.xlsx
+++ b/quickstart/jsonbox_test_api_just_wrapper.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Base_Config" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
   <si>
     <t xml:space="preserve">app_name</t>
   </si>
@@ -118,41 +118,11 @@
     "username": "kannanr",
     "email": "kannan@techconative.com"
   },
-  "read_expected_response": "${read_exec_secnario.create_entry.request}"
+  "read_expected_response": "${read_exec_scenario.create_entry.request}"
 }</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">delete_exec_scenario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete newly created user and validate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">create_entry,read_entry_200,delete_entry,read_entry_500</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">create_entry_scenario,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">read_exec_scenario</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">test_api_wrapper_name</t>
@@ -165,36 +135,6 @@
   </si>
   <si>
     <t xml:space="preserve">test_api_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">read_entry_200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User retrieval success</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"expected_read_status_code": "200"}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">read_entry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">read_entry_404</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User not found</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"expected_read_status_code": "404"}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">read_entry_500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User retrieval failed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"expected_read_status_code": "500"}</t>
   </si>
   <si>
     <t xml:space="preserve">api_unique_name</t>
@@ -269,6 +209,9 @@
     <t xml:space="preserve">NOOP_MATCHER</t>
   </si>
   <si>
+    <t xml:space="preserve">read_entry</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reads an entry from the jsonbox.</t>
   </si>
   <si>
@@ -299,7 +242,7 @@
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="166" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -359,12 +302,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
     <font>
       <strike val="true"/>
@@ -459,7 +396,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -532,19 +469,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -560,7 +489,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -569,6 +498,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -612,10 +545,10 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="1" sqref="K3 E9"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.17578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.6"/>
@@ -3658,10 +3591,10 @@
   <dimension ref="A1:Y994"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="K3 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.17578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.2"/>
@@ -6707,13 +6640,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA994"/>
+  <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="K3 A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.17578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="23"/>
@@ -6855,36 +6788,19 @@
       <c r="Z3" s="17"/>
       <c r="AA3" s="17"/>
     </row>
-    <row r="4" customFormat="false" ht="113.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>27</v>
-      </c>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="4"/>
+      <c r="F4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E5" s="4"/>
+      <c r="D5" s="18"/>
       <c r="F5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D6" s="18"/>
       <c r="F6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -6924,7 +6840,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -11824,11 +11740,7 @@
       <c r="H993" s="2"/>
       <c r="I993" s="2"/>
     </row>
-    <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F994" s="2"/>
-      <c r="H994" s="2"/>
-      <c r="I994" s="2"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -11845,13 +11757,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="K3 A1"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.98"/>
@@ -11861,58 +11773,16 @@
   <sheetData>
     <row r="1" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="19" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -11933,11 +11803,11 @@
   </sheetPr>
   <dimension ref="A1:Y994"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.17578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.4"/>
@@ -11958,49 +11828,49 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
-      <c r="G1" s="22" t="s">
-        <v>53</v>
+      <c r="G1" s="20" t="s">
+        <v>39</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
@@ -12018,3071 +11888,3071 @@
         <v>22</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E2" s="9"/>
-      <c r="F2" s="23" t="s">
-        <v>65</v>
+      <c r="F2" s="21" t="s">
+        <v>51</v>
       </c>
-      <c r="G2" s="24" t="s">
-        <v>66</v>
+      <c r="G2" s="22" t="s">
+        <v>52</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="9"/>
-      <c r="J2" s="23" t="s">
-        <v>67</v>
+      <c r="J2" s="21" t="s">
+        <v>53</v>
       </c>
-      <c r="K2" s="25" t="s">
-        <v>68</v>
+      <c r="K2" s="23" t="s">
+        <v>54</v>
       </c>
       <c r="L2" s="9"/>
-      <c r="M2" s="25" t="s">
-        <v>69</v>
+      <c r="M2" s="23" t="s">
+        <v>55</v>
       </c>
-      <c r="N2" s="26" t="n">
+      <c r="N2" s="24" t="n">
         <v>200</v>
       </c>
-      <c r="O2" s="27"/>
+      <c r="O2" s="25"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="21" t="s">
-        <v>40</v>
+      <c r="A3" s="26" t="s">
+        <v>56</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>70</v>
+      <c r="B3" s="26" t="s">
+        <v>57</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>71</v>
+      <c r="C3" s="26" t="s">
+        <v>58</v>
       </c>
-      <c r="D3" s="21" t="s">
-        <v>72</v>
+      <c r="D3" s="26" t="s">
+        <v>59</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="G3" s="28"/>
+      <c r="G3" s="27"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
-      <c r="J3" s="29" t="s">
-        <v>73</v>
+      <c r="J3" s="28" t="s">
+        <v>60</v>
       </c>
-      <c r="K3" s="25" t="s">
-        <v>68</v>
+      <c r="K3" s="23" t="s">
+        <v>54</v>
       </c>
       <c r="L3" s="11"/>
-      <c r="M3" s="25" t="s">
-        <v>69</v>
+      <c r="M3" s="23" t="s">
+        <v>55</v>
       </c>
-      <c r="N3" s="30" t="n">
+      <c r="N3" s="29" t="n">
         <v>200</v>
       </c>
       <c r="O3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="21" t="s">
-        <v>74</v>
+      <c r="A4" s="26" t="s">
+        <v>61</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>75</v>
+      <c r="B4" s="26" t="s">
+        <v>62</v>
       </c>
-      <c r="C4" s="21" t="s">
-        <v>71</v>
+      <c r="C4" s="26" t="s">
+        <v>58</v>
       </c>
-      <c r="D4" s="21" t="s">
-        <v>76</v>
+      <c r="D4" s="26" t="s">
+        <v>63</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
-      <c r="G4" s="28"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="25" t="s">
-        <v>69</v>
+      <c r="J4" s="30"/>
+      <c r="K4" s="23" t="s">
+        <v>55</v>
       </c>
       <c r="L4" s="11"/>
-      <c r="M4" s="25" t="s">
-        <v>69</v>
+      <c r="M4" s="23" t="s">
+        <v>55</v>
       </c>
-      <c r="N4" s="30" t="n">
+      <c r="N4" s="29" t="n">
         <v>200</v>
       </c>
       <c r="O4" s="11"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G5" s="32"/>
+      <c r="G5" s="31"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G6" s="32"/>
+      <c r="G6" s="31"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G7" s="32"/>
+      <c r="G7" s="31"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G8" s="32"/>
+      <c r="G8" s="31"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G9" s="32"/>
+      <c r="G9" s="31"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G10" s="32"/>
+      <c r="G10" s="31"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G11" s="32"/>
+      <c r="G11" s="31"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G12" s="32"/>
+      <c r="G12" s="31"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G13" s="32"/>
+      <c r="G13" s="31"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G14" s="32"/>
+      <c r="G14" s="31"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G15" s="32"/>
+      <c r="G15" s="31"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G16" s="32"/>
+      <c r="G16" s="31"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G17" s="32"/>
+      <c r="G17" s="31"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G18" s="32"/>
+      <c r="G18" s="31"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G19" s="32"/>
+      <c r="G19" s="31"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G20" s="32"/>
+      <c r="G20" s="31"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G21" s="32"/>
+      <c r="G21" s="31"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G22" s="32"/>
+      <c r="G22" s="31"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G23" s="32"/>
+      <c r="G23" s="31"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G24" s="32"/>
+      <c r="G24" s="31"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G25" s="32"/>
+      <c r="G25" s="31"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G26" s="32"/>
+      <c r="G26" s="31"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G27" s="32"/>
+      <c r="G27" s="31"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G28" s="32"/>
+      <c r="G28" s="31"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G29" s="32"/>
+      <c r="G29" s="31"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G30" s="32"/>
+      <c r="G30" s="31"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G31" s="32"/>
+      <c r="G31" s="31"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G32" s="32"/>
+      <c r="G32" s="31"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G33" s="32"/>
+      <c r="G33" s="31"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G34" s="32"/>
+      <c r="G34" s="31"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G35" s="32"/>
+      <c r="G35" s="31"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G36" s="32"/>
+      <c r="G36" s="31"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G37" s="32"/>
+      <c r="G37" s="31"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G38" s="32"/>
+      <c r="G38" s="31"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G39" s="32"/>
+      <c r="G39" s="31"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G40" s="32"/>
+      <c r="G40" s="31"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G41" s="32"/>
+      <c r="G41" s="31"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G42" s="32"/>
+      <c r="G42" s="31"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G43" s="32"/>
+      <c r="G43" s="31"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G44" s="32"/>
+      <c r="G44" s="31"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G45" s="32"/>
+      <c r="G45" s="31"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G46" s="32"/>
+      <c r="G46" s="31"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G47" s="32"/>
+      <c r="G47" s="31"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G48" s="32"/>
+      <c r="G48" s="31"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G49" s="32"/>
+      <c r="G49" s="31"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G50" s="32"/>
+      <c r="G50" s="31"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G51" s="32"/>
+      <c r="G51" s="31"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G52" s="32"/>
+      <c r="G52" s="31"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G53" s="32"/>
+      <c r="G53" s="31"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G54" s="32"/>
+      <c r="G54" s="31"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G55" s="32"/>
+      <c r="G55" s="31"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G56" s="32"/>
+      <c r="G56" s="31"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G57" s="32"/>
+      <c r="G57" s="31"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G58" s="32"/>
+      <c r="G58" s="31"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G59" s="32"/>
+      <c r="G59" s="31"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G60" s="32"/>
+      <c r="G60" s="31"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G61" s="32"/>
+      <c r="G61" s="31"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G62" s="32"/>
+      <c r="G62" s="31"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G63" s="32"/>
+      <c r="G63" s="31"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G64" s="32"/>
+      <c r="G64" s="31"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G65" s="32"/>
+      <c r="G65" s="31"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G66" s="32"/>
+      <c r="G66" s="31"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G67" s="32"/>
+      <c r="G67" s="31"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G68" s="32"/>
+      <c r="G68" s="31"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G69" s="32"/>
+      <c r="G69" s="31"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G70" s="32"/>
+      <c r="G70" s="31"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G71" s="32"/>
+      <c r="G71" s="31"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G72" s="32"/>
+      <c r="G72" s="31"/>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G73" s="32"/>
+      <c r="G73" s="31"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G74" s="32"/>
+      <c r="G74" s="31"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G75" s="32"/>
+      <c r="G75" s="31"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G76" s="32"/>
+      <c r="G76" s="31"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G77" s="32"/>
+      <c r="G77" s="31"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G78" s="32"/>
+      <c r="G78" s="31"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G79" s="32"/>
+      <c r="G79" s="31"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G80" s="32"/>
+      <c r="G80" s="31"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G81" s="32"/>
+      <c r="G81" s="31"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G82" s="32"/>
+      <c r="G82" s="31"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G83" s="32"/>
+      <c r="G83" s="31"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G84" s="32"/>
+      <c r="G84" s="31"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G85" s="32"/>
+      <c r="G85" s="31"/>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G86" s="32"/>
+      <c r="G86" s="31"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G87" s="32"/>
+      <c r="G87" s="31"/>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G88" s="32"/>
+      <c r="G88" s="31"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G89" s="32"/>
+      <c r="G89" s="31"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G90" s="32"/>
+      <c r="G90" s="31"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G91" s="32"/>
+      <c r="G91" s="31"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G92" s="32"/>
+      <c r="G92" s="31"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G93" s="32"/>
+      <c r="G93" s="31"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G94" s="32"/>
+      <c r="G94" s="31"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G95" s="32"/>
+      <c r="G95" s="31"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G96" s="32"/>
+      <c r="G96" s="31"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G97" s="32"/>
+      <c r="G97" s="31"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G98" s="32"/>
+      <c r="G98" s="31"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G99" s="32"/>
+      <c r="G99" s="31"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G100" s="32"/>
+      <c r="G100" s="31"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G101" s="32"/>
+      <c r="G101" s="31"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G102" s="32"/>
+      <c r="G102" s="31"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G103" s="32"/>
+      <c r="G103" s="31"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G104" s="32"/>
+      <c r="G104" s="31"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G105" s="32"/>
+      <c r="G105" s="31"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G106" s="32"/>
+      <c r="G106" s="31"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G107" s="32"/>
+      <c r="G107" s="31"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G108" s="32"/>
+      <c r="G108" s="31"/>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G109" s="32"/>
+      <c r="G109" s="31"/>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G110" s="32"/>
+      <c r="G110" s="31"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G111" s="32"/>
+      <c r="G111" s="31"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G112" s="32"/>
+      <c r="G112" s="31"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G113" s="32"/>
+      <c r="G113" s="31"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G114" s="32"/>
+      <c r="G114" s="31"/>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G115" s="32"/>
+      <c r="G115" s="31"/>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G116" s="32"/>
+      <c r="G116" s="31"/>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G117" s="32"/>
+      <c r="G117" s="31"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G118" s="32"/>
+      <c r="G118" s="31"/>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G119" s="32"/>
+      <c r="G119" s="31"/>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G120" s="32"/>
+      <c r="G120" s="31"/>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G121" s="32"/>
+      <c r="G121" s="31"/>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G122" s="32"/>
+      <c r="G122" s="31"/>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G123" s="32"/>
+      <c r="G123" s="31"/>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G124" s="32"/>
+      <c r="G124" s="31"/>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G125" s="32"/>
+      <c r="G125" s="31"/>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G126" s="32"/>
+      <c r="G126" s="31"/>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G127" s="32"/>
+      <c r="G127" s="31"/>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G128" s="32"/>
+      <c r="G128" s="31"/>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G129" s="32"/>
+      <c r="G129" s="31"/>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G130" s="32"/>
+      <c r="G130" s="31"/>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G131" s="32"/>
+      <c r="G131" s="31"/>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G132" s="32"/>
+      <c r="G132" s="31"/>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G133" s="32"/>
+      <c r="G133" s="31"/>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G134" s="32"/>
+      <c r="G134" s="31"/>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G135" s="32"/>
+      <c r="G135" s="31"/>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G136" s="32"/>
+      <c r="G136" s="31"/>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G137" s="32"/>
+      <c r="G137" s="31"/>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G138" s="32"/>
+      <c r="G138" s="31"/>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G139" s="32"/>
+      <c r="G139" s="31"/>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G140" s="32"/>
+      <c r="G140" s="31"/>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G141" s="32"/>
+      <c r="G141" s="31"/>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G142" s="32"/>
+      <c r="G142" s="31"/>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G143" s="32"/>
+      <c r="G143" s="31"/>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G144" s="32"/>
+      <c r="G144" s="31"/>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G145" s="32"/>
+      <c r="G145" s="31"/>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G146" s="32"/>
+      <c r="G146" s="31"/>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G147" s="32"/>
+      <c r="G147" s="31"/>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G148" s="32"/>
+      <c r="G148" s="31"/>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G149" s="32"/>
+      <c r="G149" s="31"/>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G150" s="32"/>
+      <c r="G150" s="31"/>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G151" s="32"/>
+      <c r="G151" s="31"/>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G152" s="32"/>
+      <c r="G152" s="31"/>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G153" s="32"/>
+      <c r="G153" s="31"/>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G154" s="32"/>
+      <c r="G154" s="31"/>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G155" s="32"/>
+      <c r="G155" s="31"/>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G156" s="32"/>
+      <c r="G156" s="31"/>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G157" s="32"/>
+      <c r="G157" s="31"/>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G158" s="32"/>
+      <c r="G158" s="31"/>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G159" s="32"/>
+      <c r="G159" s="31"/>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G160" s="32"/>
+      <c r="G160" s="31"/>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G161" s="32"/>
+      <c r="G161" s="31"/>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G162" s="32"/>
+      <c r="G162" s="31"/>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G163" s="32"/>
+      <c r="G163" s="31"/>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G164" s="32"/>
+      <c r="G164" s="31"/>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G165" s="32"/>
+      <c r="G165" s="31"/>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G166" s="32"/>
+      <c r="G166" s="31"/>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G167" s="32"/>
+      <c r="G167" s="31"/>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G168" s="32"/>
+      <c r="G168" s="31"/>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G169" s="32"/>
+      <c r="G169" s="31"/>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G170" s="32"/>
+      <c r="G170" s="31"/>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G171" s="32"/>
+      <c r="G171" s="31"/>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G172" s="32"/>
+      <c r="G172" s="31"/>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G173" s="32"/>
+      <c r="G173" s="31"/>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G174" s="32"/>
+      <c r="G174" s="31"/>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G175" s="32"/>
+      <c r="G175" s="31"/>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G176" s="32"/>
+      <c r="G176" s="31"/>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G177" s="32"/>
+      <c r="G177" s="31"/>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G178" s="32"/>
+      <c r="G178" s="31"/>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G179" s="32"/>
+      <c r="G179" s="31"/>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G180" s="32"/>
+      <c r="G180" s="31"/>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G181" s="32"/>
+      <c r="G181" s="31"/>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G182" s="32"/>
+      <c r="G182" s="31"/>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G183" s="32"/>
+      <c r="G183" s="31"/>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G184" s="32"/>
+      <c r="G184" s="31"/>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G185" s="32"/>
+      <c r="G185" s="31"/>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G186" s="32"/>
+      <c r="G186" s="31"/>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G187" s="32"/>
+      <c r="G187" s="31"/>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G188" s="32"/>
+      <c r="G188" s="31"/>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G189" s="32"/>
+      <c r="G189" s="31"/>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G190" s="32"/>
+      <c r="G190" s="31"/>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G191" s="32"/>
+      <c r="G191" s="31"/>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G192" s="32"/>
+      <c r="G192" s="31"/>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G193" s="32"/>
+      <c r="G193" s="31"/>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G194" s="32"/>
+      <c r="G194" s="31"/>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G195" s="32"/>
+      <c r="G195" s="31"/>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G196" s="32"/>
+      <c r="G196" s="31"/>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G197" s="32"/>
+      <c r="G197" s="31"/>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G198" s="32"/>
+      <c r="G198" s="31"/>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G199" s="32"/>
+      <c r="G199" s="31"/>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G200" s="32"/>
+      <c r="G200" s="31"/>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G201" s="32"/>
+      <c r="G201" s="31"/>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G202" s="32"/>
+      <c r="G202" s="31"/>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G203" s="32"/>
+      <c r="G203" s="31"/>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G204" s="32"/>
+      <c r="G204" s="31"/>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G205" s="32"/>
+      <c r="G205" s="31"/>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G206" s="32"/>
+      <c r="G206" s="31"/>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G207" s="32"/>
+      <c r="G207" s="31"/>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G208" s="32"/>
+      <c r="G208" s="31"/>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G209" s="32"/>
+      <c r="G209" s="31"/>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G210" s="32"/>
+      <c r="G210" s="31"/>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G211" s="32"/>
+      <c r="G211" s="31"/>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G212" s="32"/>
+      <c r="G212" s="31"/>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G213" s="32"/>
+      <c r="G213" s="31"/>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G214" s="32"/>
+      <c r="G214" s="31"/>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G215" s="32"/>
+      <c r="G215" s="31"/>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G216" s="32"/>
+      <c r="G216" s="31"/>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G217" s="32"/>
+      <c r="G217" s="31"/>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G218" s="32"/>
+      <c r="G218" s="31"/>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G219" s="32"/>
+      <c r="G219" s="31"/>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G220" s="32"/>
+      <c r="G220" s="31"/>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G221" s="32"/>
+      <c r="G221" s="31"/>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G222" s="32"/>
+      <c r="G222" s="31"/>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G223" s="32"/>
+      <c r="G223" s="31"/>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G224" s="32"/>
+      <c r="G224" s="31"/>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G225" s="32"/>
+      <c r="G225" s="31"/>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G226" s="32"/>
+      <c r="G226" s="31"/>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G227" s="32"/>
+      <c r="G227" s="31"/>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G228" s="32"/>
+      <c r="G228" s="31"/>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G229" s="32"/>
+      <c r="G229" s="31"/>
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G230" s="32"/>
+      <c r="G230" s="31"/>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G231" s="32"/>
+      <c r="G231" s="31"/>
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G232" s="32"/>
+      <c r="G232" s="31"/>
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G233" s="32"/>
+      <c r="G233" s="31"/>
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G234" s="32"/>
+      <c r="G234" s="31"/>
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G235" s="32"/>
+      <c r="G235" s="31"/>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G236" s="32"/>
+      <c r="G236" s="31"/>
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G237" s="32"/>
+      <c r="G237" s="31"/>
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G238" s="32"/>
+      <c r="G238" s="31"/>
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G239" s="32"/>
+      <c r="G239" s="31"/>
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G240" s="32"/>
+      <c r="G240" s="31"/>
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G241" s="32"/>
+      <c r="G241" s="31"/>
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G242" s="32"/>
+      <c r="G242" s="31"/>
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G243" s="32"/>
+      <c r="G243" s="31"/>
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G244" s="32"/>
+      <c r="G244" s="31"/>
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G245" s="32"/>
+      <c r="G245" s="31"/>
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G246" s="32"/>
+      <c r="G246" s="31"/>
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G247" s="32"/>
+      <c r="G247" s="31"/>
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G248" s="32"/>
+      <c r="G248" s="31"/>
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G249" s="32"/>
+      <c r="G249" s="31"/>
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G250" s="32"/>
+      <c r="G250" s="31"/>
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G251" s="32"/>
+      <c r="G251" s="31"/>
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G252" s="32"/>
+      <c r="G252" s="31"/>
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G253" s="32"/>
+      <c r="G253" s="31"/>
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G254" s="32"/>
+      <c r="G254" s="31"/>
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G255" s="32"/>
+      <c r="G255" s="31"/>
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G256" s="32"/>
+      <c r="G256" s="31"/>
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G257" s="32"/>
+      <c r="G257" s="31"/>
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G258" s="32"/>
+      <c r="G258" s="31"/>
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G259" s="32"/>
+      <c r="G259" s="31"/>
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G260" s="32"/>
+      <c r="G260" s="31"/>
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G261" s="32"/>
+      <c r="G261" s="31"/>
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G262" s="32"/>
+      <c r="G262" s="31"/>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G263" s="32"/>
+      <c r="G263" s="31"/>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G264" s="32"/>
+      <c r="G264" s="31"/>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G265" s="32"/>
+      <c r="G265" s="31"/>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G266" s="32"/>
+      <c r="G266" s="31"/>
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G267" s="32"/>
+      <c r="G267" s="31"/>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G268" s="32"/>
+      <c r="G268" s="31"/>
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G269" s="32"/>
+      <c r="G269" s="31"/>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G270" s="32"/>
+      <c r="G270" s="31"/>
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G271" s="32"/>
+      <c r="G271" s="31"/>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G272" s="32"/>
+      <c r="G272" s="31"/>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G273" s="32"/>
+      <c r="G273" s="31"/>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G274" s="32"/>
+      <c r="G274" s="31"/>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G275" s="32"/>
+      <c r="G275" s="31"/>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G276" s="32"/>
+      <c r="G276" s="31"/>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G277" s="32"/>
+      <c r="G277" s="31"/>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G278" s="32"/>
+      <c r="G278" s="31"/>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G279" s="32"/>
+      <c r="G279" s="31"/>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G280" s="32"/>
+      <c r="G280" s="31"/>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G281" s="32"/>
+      <c r="G281" s="31"/>
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G282" s="32"/>
+      <c r="G282" s="31"/>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G283" s="32"/>
+      <c r="G283" s="31"/>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G284" s="32"/>
+      <c r="G284" s="31"/>
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G285" s="32"/>
+      <c r="G285" s="31"/>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G286" s="32"/>
+      <c r="G286" s="31"/>
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G287" s="32"/>
+      <c r="G287" s="31"/>
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G288" s="32"/>
+      <c r="G288" s="31"/>
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G289" s="32"/>
+      <c r="G289" s="31"/>
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G290" s="32"/>
+      <c r="G290" s="31"/>
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G291" s="32"/>
+      <c r="G291" s="31"/>
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G292" s="32"/>
+      <c r="G292" s="31"/>
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G293" s="32"/>
+      <c r="G293" s="31"/>
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G294" s="32"/>
+      <c r="G294" s="31"/>
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G295" s="32"/>
+      <c r="G295" s="31"/>
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G296" s="32"/>
+      <c r="G296" s="31"/>
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G297" s="32"/>
+      <c r="G297" s="31"/>
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G298" s="32"/>
+      <c r="G298" s="31"/>
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G299" s="32"/>
+      <c r="G299" s="31"/>
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G300" s="32"/>
+      <c r="G300" s="31"/>
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G301" s="32"/>
+      <c r="G301" s="31"/>
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G302" s="32"/>
+      <c r="G302" s="31"/>
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G303" s="32"/>
+      <c r="G303" s="31"/>
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G304" s="32"/>
+      <c r="G304" s="31"/>
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G305" s="32"/>
+      <c r="G305" s="31"/>
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G306" s="32"/>
+      <c r="G306" s="31"/>
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G307" s="32"/>
+      <c r="G307" s="31"/>
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G308" s="32"/>
+      <c r="G308" s="31"/>
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G309" s="32"/>
+      <c r="G309" s="31"/>
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G310" s="32"/>
+      <c r="G310" s="31"/>
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G311" s="32"/>
+      <c r="G311" s="31"/>
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G312" s="32"/>
+      <c r="G312" s="31"/>
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G313" s="32"/>
+      <c r="G313" s="31"/>
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G314" s="32"/>
+      <c r="G314" s="31"/>
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G315" s="32"/>
+      <c r="G315" s="31"/>
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G316" s="32"/>
+      <c r="G316" s="31"/>
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G317" s="32"/>
+      <c r="G317" s="31"/>
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G318" s="32"/>
+      <c r="G318" s="31"/>
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G319" s="32"/>
+      <c r="G319" s="31"/>
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G320" s="32"/>
+      <c r="G320" s="31"/>
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G321" s="32"/>
+      <c r="G321" s="31"/>
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G322" s="32"/>
+      <c r="G322" s="31"/>
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G323" s="32"/>
+      <c r="G323" s="31"/>
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G324" s="32"/>
+      <c r="G324" s="31"/>
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G325" s="32"/>
+      <c r="G325" s="31"/>
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G326" s="32"/>
+      <c r="G326" s="31"/>
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G327" s="32"/>
+      <c r="G327" s="31"/>
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G328" s="32"/>
+      <c r="G328" s="31"/>
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G329" s="32"/>
+      <c r="G329" s="31"/>
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G330" s="32"/>
+      <c r="G330" s="31"/>
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G331" s="32"/>
+      <c r="G331" s="31"/>
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G332" s="32"/>
+      <c r="G332" s="31"/>
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G333" s="32"/>
+      <c r="G333" s="31"/>
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G334" s="32"/>
+      <c r="G334" s="31"/>
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G335" s="32"/>
+      <c r="G335" s="31"/>
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G336" s="32"/>
+      <c r="G336" s="31"/>
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G337" s="32"/>
+      <c r="G337" s="31"/>
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G338" s="32"/>
+      <c r="G338" s="31"/>
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G339" s="32"/>
+      <c r="G339" s="31"/>
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G340" s="32"/>
+      <c r="G340" s="31"/>
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G341" s="32"/>
+      <c r="G341" s="31"/>
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G342" s="32"/>
+      <c r="G342" s="31"/>
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G343" s="32"/>
+      <c r="G343" s="31"/>
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G344" s="32"/>
+      <c r="G344" s="31"/>
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G345" s="32"/>
+      <c r="G345" s="31"/>
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G346" s="32"/>
+      <c r="G346" s="31"/>
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G347" s="32"/>
+      <c r="G347" s="31"/>
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G348" s="32"/>
+      <c r="G348" s="31"/>
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G349" s="32"/>
+      <c r="G349" s="31"/>
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G350" s="32"/>
+      <c r="G350" s="31"/>
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G351" s="32"/>
+      <c r="G351" s="31"/>
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G352" s="32"/>
+      <c r="G352" s="31"/>
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G353" s="32"/>
+      <c r="G353" s="31"/>
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G354" s="32"/>
+      <c r="G354" s="31"/>
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G355" s="32"/>
+      <c r="G355" s="31"/>
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G356" s="32"/>
+      <c r="G356" s="31"/>
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G357" s="32"/>
+      <c r="G357" s="31"/>
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G358" s="32"/>
+      <c r="G358" s="31"/>
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G359" s="32"/>
+      <c r="G359" s="31"/>
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G360" s="32"/>
+      <c r="G360" s="31"/>
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G361" s="32"/>
+      <c r="G361" s="31"/>
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G362" s="32"/>
+      <c r="G362" s="31"/>
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G363" s="32"/>
+      <c r="G363" s="31"/>
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G364" s="32"/>
+      <c r="G364" s="31"/>
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G365" s="32"/>
+      <c r="G365" s="31"/>
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G366" s="32"/>
+      <c r="G366" s="31"/>
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G367" s="32"/>
+      <c r="G367" s="31"/>
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G368" s="32"/>
+      <c r="G368" s="31"/>
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G369" s="32"/>
+      <c r="G369" s="31"/>
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G370" s="32"/>
+      <c r="G370" s="31"/>
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G371" s="32"/>
+      <c r="G371" s="31"/>
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G372" s="32"/>
+      <c r="G372" s="31"/>
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G373" s="32"/>
+      <c r="G373" s="31"/>
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G374" s="32"/>
+      <c r="G374" s="31"/>
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G375" s="32"/>
+      <c r="G375" s="31"/>
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G376" s="32"/>
+      <c r="G376" s="31"/>
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G377" s="32"/>
+      <c r="G377" s="31"/>
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G378" s="32"/>
+      <c r="G378" s="31"/>
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G379" s="32"/>
+      <c r="G379" s="31"/>
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G380" s="32"/>
+      <c r="G380" s="31"/>
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G381" s="32"/>
+      <c r="G381" s="31"/>
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G382" s="32"/>
+      <c r="G382" s="31"/>
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G383" s="32"/>
+      <c r="G383" s="31"/>
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G384" s="32"/>
+      <c r="G384" s="31"/>
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G385" s="32"/>
+      <c r="G385" s="31"/>
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G386" s="32"/>
+      <c r="G386" s="31"/>
     </row>
     <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G387" s="32"/>
+      <c r="G387" s="31"/>
     </row>
     <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G388" s="32"/>
+      <c r="G388" s="31"/>
     </row>
     <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G389" s="32"/>
+      <c r="G389" s="31"/>
     </row>
     <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G390" s="32"/>
+      <c r="G390" s="31"/>
     </row>
     <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G391" s="32"/>
+      <c r="G391" s="31"/>
     </row>
     <row r="392" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G392" s="32"/>
+      <c r="G392" s="31"/>
     </row>
     <row r="393" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G393" s="32"/>
+      <c r="G393" s="31"/>
     </row>
     <row r="394" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G394" s="32"/>
+      <c r="G394" s="31"/>
     </row>
     <row r="395" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G395" s="32"/>
+      <c r="G395" s="31"/>
     </row>
     <row r="396" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G396" s="32"/>
+      <c r="G396" s="31"/>
     </row>
     <row r="397" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G397" s="32"/>
+      <c r="G397" s="31"/>
     </row>
     <row r="398" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G398" s="32"/>
+      <c r="G398" s="31"/>
     </row>
     <row r="399" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G399" s="32"/>
+      <c r="G399" s="31"/>
     </row>
     <row r="400" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G400" s="32"/>
+      <c r="G400" s="31"/>
     </row>
     <row r="401" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G401" s="32"/>
+      <c r="G401" s="31"/>
     </row>
     <row r="402" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G402" s="32"/>
+      <c r="G402" s="31"/>
     </row>
     <row r="403" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G403" s="32"/>
+      <c r="G403" s="31"/>
     </row>
     <row r="404" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G404" s="32"/>
+      <c r="G404" s="31"/>
     </row>
     <row r="405" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G405" s="32"/>
+      <c r="G405" s="31"/>
     </row>
     <row r="406" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G406" s="32"/>
+      <c r="G406" s="31"/>
     </row>
     <row r="407" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G407" s="32"/>
+      <c r="G407" s="31"/>
     </row>
     <row r="408" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G408" s="32"/>
+      <c r="G408" s="31"/>
     </row>
     <row r="409" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G409" s="32"/>
+      <c r="G409" s="31"/>
     </row>
     <row r="410" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G410" s="32"/>
+      <c r="G410" s="31"/>
     </row>
     <row r="411" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G411" s="32"/>
+      <c r="G411" s="31"/>
     </row>
     <row r="412" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G412" s="32"/>
+      <c r="G412" s="31"/>
     </row>
     <row r="413" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G413" s="32"/>
+      <c r="G413" s="31"/>
     </row>
     <row r="414" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G414" s="32"/>
+      <c r="G414" s="31"/>
     </row>
     <row r="415" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G415" s="32"/>
+      <c r="G415" s="31"/>
     </row>
     <row r="416" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G416" s="32"/>
+      <c r="G416" s="31"/>
     </row>
     <row r="417" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G417" s="32"/>
+      <c r="G417" s="31"/>
     </row>
     <row r="418" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G418" s="32"/>
+      <c r="G418" s="31"/>
     </row>
     <row r="419" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G419" s="32"/>
+      <c r="G419" s="31"/>
     </row>
     <row r="420" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G420" s="32"/>
+      <c r="G420" s="31"/>
     </row>
     <row r="421" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G421" s="32"/>
+      <c r="G421" s="31"/>
     </row>
     <row r="422" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G422" s="32"/>
+      <c r="G422" s="31"/>
     </row>
     <row r="423" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G423" s="32"/>
+      <c r="G423" s="31"/>
     </row>
     <row r="424" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G424" s="32"/>
+      <c r="G424" s="31"/>
     </row>
     <row r="425" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G425" s="32"/>
+      <c r="G425" s="31"/>
     </row>
     <row r="426" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G426" s="32"/>
+      <c r="G426" s="31"/>
     </row>
     <row r="427" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G427" s="32"/>
+      <c r="G427" s="31"/>
     </row>
     <row r="428" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G428" s="32"/>
+      <c r="G428" s="31"/>
     </row>
     <row r="429" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G429" s="32"/>
+      <c r="G429" s="31"/>
     </row>
     <row r="430" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G430" s="32"/>
+      <c r="G430" s="31"/>
     </row>
     <row r="431" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G431" s="32"/>
+      <c r="G431" s="31"/>
     </row>
     <row r="432" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G432" s="32"/>
+      <c r="G432" s="31"/>
     </row>
     <row r="433" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G433" s="32"/>
+      <c r="G433" s="31"/>
     </row>
     <row r="434" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G434" s="32"/>
+      <c r="G434" s="31"/>
     </row>
     <row r="435" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G435" s="32"/>
+      <c r="G435" s="31"/>
     </row>
     <row r="436" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G436" s="32"/>
+      <c r="G436" s="31"/>
     </row>
     <row r="437" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G437" s="32"/>
+      <c r="G437" s="31"/>
     </row>
     <row r="438" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G438" s="32"/>
+      <c r="G438" s="31"/>
     </row>
     <row r="439" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G439" s="32"/>
+      <c r="G439" s="31"/>
     </row>
     <row r="440" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G440" s="32"/>
+      <c r="G440" s="31"/>
     </row>
     <row r="441" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G441" s="32"/>
+      <c r="G441" s="31"/>
     </row>
     <row r="442" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G442" s="32"/>
+      <c r="G442" s="31"/>
     </row>
     <row r="443" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G443" s="32"/>
+      <c r="G443" s="31"/>
     </row>
     <row r="444" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G444" s="32"/>
+      <c r="G444" s="31"/>
     </row>
     <row r="445" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G445" s="32"/>
+      <c r="G445" s="31"/>
     </row>
     <row r="446" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G446" s="32"/>
+      <c r="G446" s="31"/>
     </row>
     <row r="447" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G447" s="32"/>
+      <c r="G447" s="31"/>
     </row>
     <row r="448" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G448" s="32"/>
+      <c r="G448" s="31"/>
     </row>
     <row r="449" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G449" s="32"/>
+      <c r="G449" s="31"/>
     </row>
     <row r="450" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G450" s="32"/>
+      <c r="G450" s="31"/>
     </row>
     <row r="451" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G451" s="32"/>
+      <c r="G451" s="31"/>
     </row>
     <row r="452" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G452" s="32"/>
+      <c r="G452" s="31"/>
     </row>
     <row r="453" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G453" s="32"/>
+      <c r="G453" s="31"/>
     </row>
     <row r="454" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G454" s="32"/>
+      <c r="G454" s="31"/>
     </row>
     <row r="455" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G455" s="32"/>
+      <c r="G455" s="31"/>
     </row>
     <row r="456" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G456" s="32"/>
+      <c r="G456" s="31"/>
     </row>
     <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G457" s="32"/>
+      <c r="G457" s="31"/>
     </row>
     <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G458" s="32"/>
+      <c r="G458" s="31"/>
     </row>
     <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G459" s="32"/>
+      <c r="G459" s="31"/>
     </row>
     <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G460" s="32"/>
+      <c r="G460" s="31"/>
     </row>
     <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G461" s="32"/>
+      <c r="G461" s="31"/>
     </row>
     <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G462" s="32"/>
+      <c r="G462" s="31"/>
     </row>
     <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G463" s="32"/>
+      <c r="G463" s="31"/>
     </row>
     <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G464" s="32"/>
+      <c r="G464" s="31"/>
     </row>
     <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G465" s="32"/>
+      <c r="G465" s="31"/>
     </row>
     <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G466" s="32"/>
+      <c r="G466" s="31"/>
     </row>
     <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G467" s="32"/>
+      <c r="G467" s="31"/>
     </row>
     <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G468" s="32"/>
+      <c r="G468" s="31"/>
     </row>
     <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G469" s="32"/>
+      <c r="G469" s="31"/>
     </row>
     <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G470" s="32"/>
+      <c r="G470" s="31"/>
     </row>
     <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G471" s="32"/>
+      <c r="G471" s="31"/>
     </row>
     <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G472" s="32"/>
+      <c r="G472" s="31"/>
     </row>
     <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G473" s="32"/>
+      <c r="G473" s="31"/>
     </row>
     <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G474" s="32"/>
+      <c r="G474" s="31"/>
     </row>
     <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G475" s="32"/>
+      <c r="G475" s="31"/>
     </row>
     <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G476" s="32"/>
+      <c r="G476" s="31"/>
     </row>
     <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G477" s="32"/>
+      <c r="G477" s="31"/>
     </row>
     <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G478" s="32"/>
+      <c r="G478" s="31"/>
     </row>
     <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G479" s="32"/>
+      <c r="G479" s="31"/>
     </row>
     <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G480" s="32"/>
+      <c r="G480" s="31"/>
     </row>
     <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G481" s="32"/>
+      <c r="G481" s="31"/>
     </row>
     <row r="482" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G482" s="32"/>
+      <c r="G482" s="31"/>
     </row>
     <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G483" s="32"/>
+      <c r="G483" s="31"/>
     </row>
     <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G484" s="32"/>
+      <c r="G484" s="31"/>
     </row>
     <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G485" s="32"/>
+      <c r="G485" s="31"/>
     </row>
     <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G486" s="32"/>
+      <c r="G486" s="31"/>
     </row>
     <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G487" s="32"/>
+      <c r="G487" s="31"/>
     </row>
     <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G488" s="32"/>
+      <c r="G488" s="31"/>
     </row>
     <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G489" s="32"/>
+      <c r="G489" s="31"/>
     </row>
     <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G490" s="32"/>
+      <c r="G490" s="31"/>
     </row>
     <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G491" s="32"/>
+      <c r="G491" s="31"/>
     </row>
     <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G492" s="32"/>
+      <c r="G492" s="31"/>
     </row>
     <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G493" s="32"/>
+      <c r="G493" s="31"/>
     </row>
     <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G494" s="32"/>
+      <c r="G494" s="31"/>
     </row>
     <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G495" s="32"/>
+      <c r="G495" s="31"/>
     </row>
     <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G496" s="32"/>
+      <c r="G496" s="31"/>
     </row>
     <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G497" s="32"/>
+      <c r="G497" s="31"/>
     </row>
     <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G498" s="32"/>
+      <c r="G498" s="31"/>
     </row>
     <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G499" s="32"/>
+      <c r="G499" s="31"/>
     </row>
     <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G500" s="32"/>
+      <c r="G500" s="31"/>
     </row>
     <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G501" s="32"/>
+      <c r="G501" s="31"/>
     </row>
     <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G502" s="32"/>
+      <c r="G502" s="31"/>
     </row>
     <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G503" s="32"/>
+      <c r="G503" s="31"/>
     </row>
     <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G504" s="32"/>
+      <c r="G504" s="31"/>
     </row>
     <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G505" s="32"/>
+      <c r="G505" s="31"/>
     </row>
     <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G506" s="32"/>
+      <c r="G506" s="31"/>
     </row>
     <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G507" s="32"/>
+      <c r="G507" s="31"/>
     </row>
     <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G508" s="32"/>
+      <c r="G508" s="31"/>
     </row>
     <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G509" s="32"/>
+      <c r="G509" s="31"/>
     </row>
     <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G510" s="32"/>
+      <c r="G510" s="31"/>
     </row>
     <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G511" s="32"/>
+      <c r="G511" s="31"/>
     </row>
     <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G512" s="32"/>
+      <c r="G512" s="31"/>
     </row>
     <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G513" s="32"/>
+      <c r="G513" s="31"/>
     </row>
     <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G514" s="32"/>
+      <c r="G514" s="31"/>
     </row>
     <row r="515" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G515" s="32"/>
+      <c r="G515" s="31"/>
     </row>
     <row r="516" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G516" s="32"/>
+      <c r="G516" s="31"/>
     </row>
     <row r="517" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G517" s="32"/>
+      <c r="G517" s="31"/>
     </row>
     <row r="518" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G518" s="32"/>
+      <c r="G518" s="31"/>
     </row>
     <row r="519" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G519" s="32"/>
+      <c r="G519" s="31"/>
     </row>
     <row r="520" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G520" s="32"/>
+      <c r="G520" s="31"/>
     </row>
     <row r="521" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G521" s="32"/>
+      <c r="G521" s="31"/>
     </row>
     <row r="522" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G522" s="32"/>
+      <c r="G522" s="31"/>
     </row>
     <row r="523" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G523" s="32"/>
+      <c r="G523" s="31"/>
     </row>
     <row r="524" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G524" s="32"/>
+      <c r="G524" s="31"/>
     </row>
     <row r="525" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G525" s="32"/>
+      <c r="G525" s="31"/>
     </row>
     <row r="526" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G526" s="32"/>
+      <c r="G526" s="31"/>
     </row>
     <row r="527" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G527" s="32"/>
+      <c r="G527" s="31"/>
     </row>
     <row r="528" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G528" s="32"/>
+      <c r="G528" s="31"/>
     </row>
     <row r="529" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G529" s="32"/>
+      <c r="G529" s="31"/>
     </row>
     <row r="530" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G530" s="32"/>
+      <c r="G530" s="31"/>
     </row>
     <row r="531" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G531" s="32"/>
+      <c r="G531" s="31"/>
     </row>
     <row r="532" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G532" s="32"/>
+      <c r="G532" s="31"/>
     </row>
     <row r="533" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G533" s="32"/>
+      <c r="G533" s="31"/>
     </row>
     <row r="534" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G534" s="32"/>
+      <c r="G534" s="31"/>
     </row>
     <row r="535" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G535" s="32"/>
+      <c r="G535" s="31"/>
     </row>
     <row r="536" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G536" s="32"/>
+      <c r="G536" s="31"/>
     </row>
     <row r="537" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G537" s="32"/>
+      <c r="G537" s="31"/>
     </row>
     <row r="538" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G538" s="32"/>
+      <c r="G538" s="31"/>
     </row>
     <row r="539" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G539" s="32"/>
+      <c r="G539" s="31"/>
     </row>
     <row r="540" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G540" s="32"/>
+      <c r="G540" s="31"/>
     </row>
     <row r="541" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G541" s="32"/>
+      <c r="G541" s="31"/>
     </row>
     <row r="542" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G542" s="32"/>
+      <c r="G542" s="31"/>
     </row>
     <row r="543" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G543" s="32"/>
+      <c r="G543" s="31"/>
     </row>
     <row r="544" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G544" s="32"/>
+      <c r="G544" s="31"/>
     </row>
     <row r="545" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G545" s="32"/>
+      <c r="G545" s="31"/>
     </row>
     <row r="546" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G546" s="32"/>
+      <c r="G546" s="31"/>
     </row>
     <row r="547" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G547" s="32"/>
+      <c r="G547" s="31"/>
     </row>
     <row r="548" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G548" s="32"/>
+      <c r="G548" s="31"/>
     </row>
     <row r="549" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G549" s="32"/>
+      <c r="G549" s="31"/>
     </row>
     <row r="550" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G550" s="32"/>
+      <c r="G550" s="31"/>
     </row>
     <row r="551" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G551" s="32"/>
+      <c r="G551" s="31"/>
     </row>
     <row r="552" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G552" s="32"/>
+      <c r="G552" s="31"/>
     </row>
     <row r="553" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G553" s="32"/>
+      <c r="G553" s="31"/>
     </row>
     <row r="554" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G554" s="32"/>
+      <c r="G554" s="31"/>
     </row>
     <row r="555" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G555" s="32"/>
+      <c r="G555" s="31"/>
     </row>
     <row r="556" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G556" s="32"/>
+      <c r="G556" s="31"/>
     </row>
     <row r="557" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G557" s="32"/>
+      <c r="G557" s="31"/>
     </row>
     <row r="558" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G558" s="32"/>
+      <c r="G558" s="31"/>
     </row>
     <row r="559" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G559" s="32"/>
+      <c r="G559" s="31"/>
     </row>
     <row r="560" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G560" s="32"/>
+      <c r="G560" s="31"/>
     </row>
     <row r="561" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G561" s="32"/>
+      <c r="G561" s="31"/>
     </row>
     <row r="562" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G562" s="32"/>
+      <c r="G562" s="31"/>
     </row>
     <row r="563" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G563" s="32"/>
+      <c r="G563" s="31"/>
     </row>
     <row r="564" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G564" s="32"/>
+      <c r="G564" s="31"/>
     </row>
     <row r="565" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G565" s="32"/>
+      <c r="G565" s="31"/>
     </row>
     <row r="566" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G566" s="32"/>
+      <c r="G566" s="31"/>
     </row>
     <row r="567" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G567" s="32"/>
+      <c r="G567" s="31"/>
     </row>
     <row r="568" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G568" s="32"/>
+      <c r="G568" s="31"/>
     </row>
     <row r="569" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G569" s="32"/>
+      <c r="G569" s="31"/>
     </row>
     <row r="570" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G570" s="32"/>
+      <c r="G570" s="31"/>
     </row>
     <row r="571" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G571" s="32"/>
+      <c r="G571" s="31"/>
     </row>
     <row r="572" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G572" s="32"/>
+      <c r="G572" s="31"/>
     </row>
     <row r="573" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G573" s="32"/>
+      <c r="G573" s="31"/>
     </row>
     <row r="574" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G574" s="32"/>
+      <c r="G574" s="31"/>
     </row>
     <row r="575" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G575" s="32"/>
+      <c r="G575" s="31"/>
     </row>
     <row r="576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G576" s="32"/>
+      <c r="G576" s="31"/>
     </row>
     <row r="577" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G577" s="32"/>
+      <c r="G577" s="31"/>
     </row>
     <row r="578" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G578" s="32"/>
+      <c r="G578" s="31"/>
     </row>
     <row r="579" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G579" s="32"/>
+      <c r="G579" s="31"/>
     </row>
     <row r="580" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G580" s="32"/>
+      <c r="G580" s="31"/>
     </row>
     <row r="581" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G581" s="32"/>
+      <c r="G581" s="31"/>
     </row>
     <row r="582" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G582" s="32"/>
+      <c r="G582" s="31"/>
     </row>
     <row r="583" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G583" s="32"/>
+      <c r="G583" s="31"/>
     </row>
     <row r="584" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G584" s="32"/>
+      <c r="G584" s="31"/>
     </row>
     <row r="585" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G585" s="32"/>
+      <c r="G585" s="31"/>
     </row>
     <row r="586" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G586" s="32"/>
+      <c r="G586" s="31"/>
     </row>
     <row r="587" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G587" s="32"/>
+      <c r="G587" s="31"/>
     </row>
     <row r="588" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G588" s="32"/>
+      <c r="G588" s="31"/>
     </row>
     <row r="589" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G589" s="32"/>
+      <c r="G589" s="31"/>
     </row>
     <row r="590" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G590" s="32"/>
+      <c r="G590" s="31"/>
     </row>
     <row r="591" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G591" s="32"/>
+      <c r="G591" s="31"/>
     </row>
     <row r="592" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G592" s="32"/>
+      <c r="G592" s="31"/>
     </row>
     <row r="593" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G593" s="32"/>
+      <c r="G593" s="31"/>
     </row>
     <row r="594" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G594" s="32"/>
+      <c r="G594" s="31"/>
     </row>
     <row r="595" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G595" s="32"/>
+      <c r="G595" s="31"/>
     </row>
     <row r="596" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G596" s="32"/>
+      <c r="G596" s="31"/>
     </row>
     <row r="597" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G597" s="32"/>
+      <c r="G597" s="31"/>
     </row>
     <row r="598" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G598" s="32"/>
+      <c r="G598" s="31"/>
     </row>
     <row r="599" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G599" s="32"/>
+      <c r="G599" s="31"/>
     </row>
     <row r="600" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G600" s="32"/>
+      <c r="G600" s="31"/>
     </row>
     <row r="601" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G601" s="32"/>
+      <c r="G601" s="31"/>
     </row>
     <row r="602" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G602" s="32"/>
+      <c r="G602" s="31"/>
     </row>
     <row r="603" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G603" s="32"/>
+      <c r="G603" s="31"/>
     </row>
     <row r="604" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G604" s="32"/>
+      <c r="G604" s="31"/>
     </row>
     <row r="605" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G605" s="32"/>
+      <c r="G605" s="31"/>
     </row>
     <row r="606" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G606" s="32"/>
+      <c r="G606" s="31"/>
     </row>
     <row r="607" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G607" s="32"/>
+      <c r="G607" s="31"/>
     </row>
     <row r="608" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G608" s="32"/>
+      <c r="G608" s="31"/>
     </row>
     <row r="609" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G609" s="32"/>
+      <c r="G609" s="31"/>
     </row>
     <row r="610" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G610" s="32"/>
+      <c r="G610" s="31"/>
     </row>
     <row r="611" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G611" s="32"/>
+      <c r="G611" s="31"/>
     </row>
     <row r="612" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G612" s="32"/>
+      <c r="G612" s="31"/>
     </row>
     <row r="613" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G613" s="32"/>
+      <c r="G613" s="31"/>
     </row>
     <row r="614" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G614" s="32"/>
+      <c r="G614" s="31"/>
     </row>
     <row r="615" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G615" s="32"/>
+      <c r="G615" s="31"/>
     </row>
     <row r="616" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G616" s="32"/>
+      <c r="G616" s="31"/>
     </row>
     <row r="617" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G617" s="32"/>
+      <c r="G617" s="31"/>
     </row>
     <row r="618" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G618" s="32"/>
+      <c r="G618" s="31"/>
     </row>
     <row r="619" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G619" s="32"/>
+      <c r="G619" s="31"/>
     </row>
     <row r="620" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G620" s="32"/>
+      <c r="G620" s="31"/>
     </row>
     <row r="621" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G621" s="32"/>
+      <c r="G621" s="31"/>
     </row>
     <row r="622" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G622" s="32"/>
+      <c r="G622" s="31"/>
     </row>
     <row r="623" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G623" s="32"/>
+      <c r="G623" s="31"/>
     </row>
     <row r="624" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G624" s="32"/>
+      <c r="G624" s="31"/>
     </row>
     <row r="625" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G625" s="32"/>
+      <c r="G625" s="31"/>
     </row>
     <row r="626" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G626" s="32"/>
+      <c r="G626" s="31"/>
     </row>
     <row r="627" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G627" s="32"/>
+      <c r="G627" s="31"/>
     </row>
     <row r="628" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G628" s="32"/>
+      <c r="G628" s="31"/>
     </row>
     <row r="629" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G629" s="32"/>
+      <c r="G629" s="31"/>
     </row>
     <row r="630" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G630" s="32"/>
+      <c r="G630" s="31"/>
     </row>
     <row r="631" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G631" s="32"/>
+      <c r="G631" s="31"/>
     </row>
     <row r="632" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G632" s="32"/>
+      <c r="G632" s="31"/>
     </row>
     <row r="633" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G633" s="32"/>
+      <c r="G633" s="31"/>
     </row>
     <row r="634" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G634" s="32"/>
+      <c r="G634" s="31"/>
     </row>
     <row r="635" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G635" s="32"/>
+      <c r="G635" s="31"/>
     </row>
     <row r="636" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G636" s="32"/>
+      <c r="G636" s="31"/>
     </row>
     <row r="637" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G637" s="32"/>
+      <c r="G637" s="31"/>
     </row>
     <row r="638" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G638" s="32"/>
+      <c r="G638" s="31"/>
     </row>
     <row r="639" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G639" s="32"/>
+      <c r="G639" s="31"/>
     </row>
     <row r="640" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G640" s="32"/>
+      <c r="G640" s="31"/>
     </row>
     <row r="641" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G641" s="32"/>
+      <c r="G641" s="31"/>
     </row>
     <row r="642" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G642" s="32"/>
+      <c r="G642" s="31"/>
     </row>
     <row r="643" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G643" s="32"/>
+      <c r="G643" s="31"/>
     </row>
     <row r="644" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G644" s="32"/>
+      <c r="G644" s="31"/>
     </row>
     <row r="645" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G645" s="32"/>
+      <c r="G645" s="31"/>
     </row>
     <row r="646" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G646" s="32"/>
+      <c r="G646" s="31"/>
     </row>
     <row r="647" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G647" s="32"/>
+      <c r="G647" s="31"/>
     </row>
     <row r="648" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G648" s="32"/>
+      <c r="G648" s="31"/>
     </row>
     <row r="649" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G649" s="32"/>
+      <c r="G649" s="31"/>
     </row>
     <row r="650" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G650" s="32"/>
+      <c r="G650" s="31"/>
     </row>
     <row r="651" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G651" s="32"/>
+      <c r="G651" s="31"/>
     </row>
     <row r="652" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G652" s="32"/>
+      <c r="G652" s="31"/>
     </row>
     <row r="653" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G653" s="32"/>
+      <c r="G653" s="31"/>
     </row>
     <row r="654" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G654" s="32"/>
+      <c r="G654" s="31"/>
     </row>
     <row r="655" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G655" s="32"/>
+      <c r="G655" s="31"/>
     </row>
     <row r="656" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G656" s="32"/>
+      <c r="G656" s="31"/>
     </row>
     <row r="657" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G657" s="32"/>
+      <c r="G657" s="31"/>
     </row>
     <row r="658" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G658" s="32"/>
+      <c r="G658" s="31"/>
     </row>
     <row r="659" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G659" s="32"/>
+      <c r="G659" s="31"/>
     </row>
     <row r="660" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G660" s="32"/>
+      <c r="G660" s="31"/>
     </row>
     <row r="661" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G661" s="32"/>
+      <c r="G661" s="31"/>
     </row>
     <row r="662" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G662" s="32"/>
+      <c r="G662" s="31"/>
     </row>
     <row r="663" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G663" s="32"/>
+      <c r="G663" s="31"/>
     </row>
     <row r="664" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G664" s="32"/>
+      <c r="G664" s="31"/>
     </row>
     <row r="665" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G665" s="32"/>
+      <c r="G665" s="31"/>
     </row>
     <row r="666" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G666" s="32"/>
+      <c r="G666" s="31"/>
     </row>
     <row r="667" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G667" s="32"/>
+      <c r="G667" s="31"/>
     </row>
     <row r="668" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G668" s="32"/>
+      <c r="G668" s="31"/>
     </row>
     <row r="669" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G669" s="32"/>
+      <c r="G669" s="31"/>
     </row>
     <row r="670" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G670" s="32"/>
+      <c r="G670" s="31"/>
     </row>
     <row r="671" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G671" s="32"/>
+      <c r="G671" s="31"/>
     </row>
     <row r="672" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G672" s="32"/>
+      <c r="G672" s="31"/>
     </row>
     <row r="673" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G673" s="32"/>
+      <c r="G673" s="31"/>
     </row>
     <row r="674" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G674" s="32"/>
+      <c r="G674" s="31"/>
     </row>
     <row r="675" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G675" s="32"/>
+      <c r="G675" s="31"/>
     </row>
     <row r="676" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G676" s="32"/>
+      <c r="G676" s="31"/>
     </row>
     <row r="677" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G677" s="32"/>
+      <c r="G677" s="31"/>
     </row>
     <row r="678" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G678" s="32"/>
+      <c r="G678" s="31"/>
     </row>
     <row r="679" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G679" s="32"/>
+      <c r="G679" s="31"/>
     </row>
     <row r="680" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G680" s="32"/>
+      <c r="G680" s="31"/>
     </row>
     <row r="681" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G681" s="32"/>
+      <c r="G681" s="31"/>
     </row>
     <row r="682" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G682" s="32"/>
+      <c r="G682" s="31"/>
     </row>
     <row r="683" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G683" s="32"/>
+      <c r="G683" s="31"/>
     </row>
     <row r="684" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G684" s="32"/>
+      <c r="G684" s="31"/>
     </row>
     <row r="685" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G685" s="32"/>
+      <c r="G685" s="31"/>
     </row>
     <row r="686" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G686" s="32"/>
+      <c r="G686" s="31"/>
     </row>
     <row r="687" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G687" s="32"/>
+      <c r="G687" s="31"/>
     </row>
     <row r="688" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G688" s="32"/>
+      <c r="G688" s="31"/>
     </row>
     <row r="689" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G689" s="32"/>
+      <c r="G689" s="31"/>
     </row>
     <row r="690" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G690" s="32"/>
+      <c r="G690" s="31"/>
     </row>
     <row r="691" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G691" s="32"/>
+      <c r="G691" s="31"/>
     </row>
     <row r="692" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G692" s="32"/>
+      <c r="G692" s="31"/>
     </row>
     <row r="693" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G693" s="32"/>
+      <c r="G693" s="31"/>
     </row>
     <row r="694" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G694" s="32"/>
+      <c r="G694" s="31"/>
     </row>
     <row r="695" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G695" s="32"/>
+      <c r="G695" s="31"/>
     </row>
     <row r="696" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G696" s="32"/>
+      <c r="G696" s="31"/>
     </row>
     <row r="697" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G697" s="32"/>
+      <c r="G697" s="31"/>
     </row>
     <row r="698" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G698" s="32"/>
+      <c r="G698" s="31"/>
     </row>
     <row r="699" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G699" s="32"/>
+      <c r="G699" s="31"/>
     </row>
     <row r="700" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G700" s="32"/>
+      <c r="G700" s="31"/>
     </row>
     <row r="701" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G701" s="32"/>
+      <c r="G701" s="31"/>
     </row>
     <row r="702" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G702" s="32"/>
+      <c r="G702" s="31"/>
     </row>
     <row r="703" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G703" s="32"/>
+      <c r="G703" s="31"/>
     </row>
     <row r="704" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G704" s="32"/>
+      <c r="G704" s="31"/>
     </row>
     <row r="705" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G705" s="32"/>
+      <c r="G705" s="31"/>
     </row>
     <row r="706" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G706" s="32"/>
+      <c r="G706" s="31"/>
     </row>
     <row r="707" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G707" s="32"/>
+      <c r="G707" s="31"/>
     </row>
     <row r="708" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G708" s="32"/>
+      <c r="G708" s="31"/>
     </row>
     <row r="709" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G709" s="32"/>
+      <c r="G709" s="31"/>
     </row>
     <row r="710" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G710" s="32"/>
+      <c r="G710" s="31"/>
     </row>
     <row r="711" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G711" s="32"/>
+      <c r="G711" s="31"/>
     </row>
     <row r="712" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G712" s="32"/>
+      <c r="G712" s="31"/>
     </row>
     <row r="713" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G713" s="32"/>
+      <c r="G713" s="31"/>
     </row>
     <row r="714" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G714" s="32"/>
+      <c r="G714" s="31"/>
     </row>
     <row r="715" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G715" s="32"/>
+      <c r="G715" s="31"/>
     </row>
     <row r="716" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G716" s="32"/>
+      <c r="G716" s="31"/>
     </row>
     <row r="717" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G717" s="32"/>
+      <c r="G717" s="31"/>
     </row>
     <row r="718" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G718" s="32"/>
+      <c r="G718" s="31"/>
     </row>
     <row r="719" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G719" s="32"/>
+      <c r="G719" s="31"/>
     </row>
     <row r="720" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G720" s="32"/>
+      <c r="G720" s="31"/>
     </row>
     <row r="721" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G721" s="32"/>
+      <c r="G721" s="31"/>
     </row>
     <row r="722" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G722" s="32"/>
+      <c r="G722" s="31"/>
     </row>
     <row r="723" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G723" s="32"/>
+      <c r="G723" s="31"/>
     </row>
     <row r="724" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G724" s="32"/>
+      <c r="G724" s="31"/>
     </row>
     <row r="725" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G725" s="32"/>
+      <c r="G725" s="31"/>
     </row>
     <row r="726" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G726" s="32"/>
+      <c r="G726" s="31"/>
     </row>
     <row r="727" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G727" s="32"/>
+      <c r="G727" s="31"/>
     </row>
     <row r="728" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G728" s="32"/>
+      <c r="G728" s="31"/>
     </row>
     <row r="729" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G729" s="32"/>
+      <c r="G729" s="31"/>
     </row>
     <row r="730" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G730" s="32"/>
+      <c r="G730" s="31"/>
     </row>
     <row r="731" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G731" s="32"/>
+      <c r="G731" s="31"/>
     </row>
     <row r="732" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G732" s="32"/>
+      <c r="G732" s="31"/>
     </row>
     <row r="733" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G733" s="32"/>
+      <c r="G733" s="31"/>
     </row>
     <row r="734" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G734" s="32"/>
+      <c r="G734" s="31"/>
     </row>
     <row r="735" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G735" s="32"/>
+      <c r="G735" s="31"/>
     </row>
     <row r="736" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G736" s="32"/>
+      <c r="G736" s="31"/>
     </row>
     <row r="737" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G737" s="32"/>
+      <c r="G737" s="31"/>
     </row>
     <row r="738" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G738" s="32"/>
+      <c r="G738" s="31"/>
     </row>
     <row r="739" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G739" s="32"/>
+      <c r="G739" s="31"/>
     </row>
     <row r="740" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G740" s="32"/>
+      <c r="G740" s="31"/>
     </row>
     <row r="741" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G741" s="32"/>
+      <c r="G741" s="31"/>
     </row>
     <row r="742" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G742" s="32"/>
+      <c r="G742" s="31"/>
     </row>
     <row r="743" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G743" s="32"/>
+      <c r="G743" s="31"/>
     </row>
     <row r="744" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G744" s="32"/>
+      <c r="G744" s="31"/>
     </row>
     <row r="745" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G745" s="32"/>
+      <c r="G745" s="31"/>
     </row>
     <row r="746" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G746" s="32"/>
+      <c r="G746" s="31"/>
     </row>
     <row r="747" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G747" s="32"/>
+      <c r="G747" s="31"/>
     </row>
     <row r="748" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G748" s="32"/>
+      <c r="G748" s="31"/>
     </row>
     <row r="749" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G749" s="32"/>
+      <c r="G749" s="31"/>
     </row>
     <row r="750" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G750" s="32"/>
+      <c r="G750" s="31"/>
     </row>
     <row r="751" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G751" s="32"/>
+      <c r="G751" s="31"/>
     </row>
     <row r="752" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G752" s="32"/>
+      <c r="G752" s="31"/>
     </row>
     <row r="753" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G753" s="32"/>
+      <c r="G753" s="31"/>
     </row>
     <row r="754" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G754" s="32"/>
+      <c r="G754" s="31"/>
     </row>
     <row r="755" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G755" s="32"/>
+      <c r="G755" s="31"/>
     </row>
     <row r="756" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G756" s="32"/>
+      <c r="G756" s="31"/>
     </row>
     <row r="757" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G757" s="32"/>
+      <c r="G757" s="31"/>
     </row>
     <row r="758" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G758" s="32"/>
+      <c r="G758" s="31"/>
     </row>
     <row r="759" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G759" s="32"/>
+      <c r="G759" s="31"/>
     </row>
     <row r="760" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G760" s="32"/>
+      <c r="G760" s="31"/>
     </row>
     <row r="761" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G761" s="32"/>
+      <c r="G761" s="31"/>
     </row>
     <row r="762" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G762" s="32"/>
+      <c r="G762" s="31"/>
     </row>
     <row r="763" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G763" s="32"/>
+      <c r="G763" s="31"/>
     </row>
     <row r="764" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G764" s="32"/>
+      <c r="G764" s="31"/>
     </row>
     <row r="765" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G765" s="32"/>
+      <c r="G765" s="31"/>
     </row>
     <row r="766" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G766" s="32"/>
+      <c r="G766" s="31"/>
     </row>
     <row r="767" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G767" s="32"/>
+      <c r="G767" s="31"/>
     </row>
     <row r="768" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G768" s="32"/>
+      <c r="G768" s="31"/>
     </row>
     <row r="769" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G769" s="32"/>
+      <c r="G769" s="31"/>
     </row>
     <row r="770" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G770" s="32"/>
+      <c r="G770" s="31"/>
     </row>
     <row r="771" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G771" s="32"/>
+      <c r="G771" s="31"/>
     </row>
     <row r="772" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G772" s="32"/>
+      <c r="G772" s="31"/>
     </row>
     <row r="773" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G773" s="32"/>
+      <c r="G773" s="31"/>
     </row>
     <row r="774" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G774" s="32"/>
+      <c r="G774" s="31"/>
     </row>
     <row r="775" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G775" s="32"/>
+      <c r="G775" s="31"/>
     </row>
     <row r="776" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G776" s="32"/>
+      <c r="G776" s="31"/>
     </row>
     <row r="777" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G777" s="32"/>
+      <c r="G777" s="31"/>
     </row>
     <row r="778" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G778" s="32"/>
+      <c r="G778" s="31"/>
     </row>
     <row r="779" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G779" s="32"/>
+      <c r="G779" s="31"/>
     </row>
     <row r="780" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G780" s="32"/>
+      <c r="G780" s="31"/>
     </row>
     <row r="781" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G781" s="32"/>
+      <c r="G781" s="31"/>
     </row>
     <row r="782" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G782" s="32"/>
+      <c r="G782" s="31"/>
     </row>
     <row r="783" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G783" s="32"/>
+      <c r="G783" s="31"/>
     </row>
     <row r="784" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G784" s="32"/>
+      <c r="G784" s="31"/>
     </row>
     <row r="785" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G785" s="32"/>
+      <c r="G785" s="31"/>
     </row>
     <row r="786" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G786" s="32"/>
+      <c r="G786" s="31"/>
     </row>
     <row r="787" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G787" s="32"/>
+      <c r="G787" s="31"/>
     </row>
     <row r="788" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G788" s="32"/>
+      <c r="G788" s="31"/>
     </row>
     <row r="789" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G789" s="32"/>
+      <c r="G789" s="31"/>
     </row>
     <row r="790" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G790" s="32"/>
+      <c r="G790" s="31"/>
     </row>
     <row r="791" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G791" s="32"/>
+      <c r="G791" s="31"/>
     </row>
     <row r="792" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G792" s="32"/>
+      <c r="G792" s="31"/>
     </row>
     <row r="793" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G793" s="32"/>
+      <c r="G793" s="31"/>
     </row>
     <row r="794" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G794" s="32"/>
+      <c r="G794" s="31"/>
     </row>
     <row r="795" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G795" s="32"/>
+      <c r="G795" s="31"/>
     </row>
     <row r="796" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G796" s="32"/>
+      <c r="G796" s="31"/>
     </row>
     <row r="797" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G797" s="32"/>
+      <c r="G797" s="31"/>
     </row>
     <row r="798" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G798" s="32"/>
+      <c r="G798" s="31"/>
     </row>
     <row r="799" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G799" s="32"/>
+      <c r="G799" s="31"/>
     </row>
     <row r="800" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G800" s="32"/>
+      <c r="G800" s="31"/>
     </row>
     <row r="801" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G801" s="32"/>
+      <c r="G801" s="31"/>
     </row>
     <row r="802" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G802" s="32"/>
+      <c r="G802" s="31"/>
     </row>
     <row r="803" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G803" s="32"/>
+      <c r="G803" s="31"/>
     </row>
     <row r="804" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G804" s="32"/>
+      <c r="G804" s="31"/>
     </row>
     <row r="805" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G805" s="32"/>
+      <c r="G805" s="31"/>
     </row>
     <row r="806" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G806" s="32"/>
+      <c r="G806" s="31"/>
     </row>
     <row r="807" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G807" s="32"/>
+      <c r="G807" s="31"/>
     </row>
     <row r="808" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G808" s="32"/>
+      <c r="G808" s="31"/>
     </row>
     <row r="809" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G809" s="32"/>
+      <c r="G809" s="31"/>
     </row>
     <row r="810" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G810" s="32"/>
+      <c r="G810" s="31"/>
     </row>
     <row r="811" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G811" s="32"/>
+      <c r="G811" s="31"/>
     </row>
     <row r="812" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G812" s="32"/>
+      <c r="G812" s="31"/>
     </row>
     <row r="813" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G813" s="32"/>
+      <c r="G813" s="31"/>
     </row>
     <row r="814" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G814" s="32"/>
+      <c r="G814" s="31"/>
     </row>
     <row r="815" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G815" s="32"/>
+      <c r="G815" s="31"/>
     </row>
     <row r="816" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G816" s="32"/>
+      <c r="G816" s="31"/>
     </row>
     <row r="817" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G817" s="32"/>
+      <c r="G817" s="31"/>
     </row>
     <row r="818" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G818" s="32"/>
+      <c r="G818" s="31"/>
     </row>
     <row r="819" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G819" s="32"/>
+      <c r="G819" s="31"/>
     </row>
     <row r="820" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G820" s="32"/>
+      <c r="G820" s="31"/>
     </row>
     <row r="821" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G821" s="32"/>
+      <c r="G821" s="31"/>
     </row>
     <row r="822" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G822" s="32"/>
+      <c r="G822" s="31"/>
     </row>
     <row r="823" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G823" s="32"/>
+      <c r="G823" s="31"/>
     </row>
     <row r="824" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G824" s="32"/>
+      <c r="G824" s="31"/>
     </row>
     <row r="825" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G825" s="32"/>
+      <c r="G825" s="31"/>
     </row>
     <row r="826" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G826" s="32"/>
+      <c r="G826" s="31"/>
     </row>
     <row r="827" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G827" s="32"/>
+      <c r="G827" s="31"/>
     </row>
     <row r="828" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G828" s="32"/>
+      <c r="G828" s="31"/>
     </row>
     <row r="829" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G829" s="32"/>
+      <c r="G829" s="31"/>
     </row>
     <row r="830" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G830" s="32"/>
+      <c r="G830" s="31"/>
     </row>
     <row r="831" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G831" s="32"/>
+      <c r="G831" s="31"/>
     </row>
     <row r="832" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G832" s="32"/>
+      <c r="G832" s="31"/>
     </row>
     <row r="833" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G833" s="32"/>
+      <c r="G833" s="31"/>
     </row>
     <row r="834" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G834" s="32"/>
+      <c r="G834" s="31"/>
     </row>
     <row r="835" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G835" s="32"/>
+      <c r="G835" s="31"/>
     </row>
     <row r="836" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G836" s="32"/>
+      <c r="G836" s="31"/>
     </row>
     <row r="837" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G837" s="32"/>
+      <c r="G837" s="31"/>
     </row>
     <row r="838" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G838" s="32"/>
+      <c r="G838" s="31"/>
     </row>
     <row r="839" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G839" s="32"/>
+      <c r="G839" s="31"/>
     </row>
     <row r="840" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G840" s="32"/>
+      <c r="G840" s="31"/>
     </row>
     <row r="841" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G841" s="32"/>
+      <c r="G841" s="31"/>
     </row>
     <row r="842" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G842" s="32"/>
+      <c r="G842" s="31"/>
     </row>
     <row r="843" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G843" s="32"/>
+      <c r="G843" s="31"/>
     </row>
     <row r="844" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G844" s="32"/>
+      <c r="G844" s="31"/>
     </row>
     <row r="845" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G845" s="32"/>
+      <c r="G845" s="31"/>
     </row>
     <row r="846" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G846" s="32"/>
+      <c r="G846" s="31"/>
     </row>
     <row r="847" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G847" s="32"/>
+      <c r="G847" s="31"/>
     </row>
     <row r="848" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G848" s="32"/>
+      <c r="G848" s="31"/>
     </row>
     <row r="849" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G849" s="32"/>
+      <c r="G849" s="31"/>
     </row>
     <row r="850" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G850" s="32"/>
+      <c r="G850" s="31"/>
     </row>
     <row r="851" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G851" s="32"/>
+      <c r="G851" s="31"/>
     </row>
     <row r="852" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G852" s="32"/>
+      <c r="G852" s="31"/>
     </row>
     <row r="853" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G853" s="32"/>
+      <c r="G853" s="31"/>
     </row>
     <row r="854" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G854" s="32"/>
+      <c r="G854" s="31"/>
     </row>
     <row r="855" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G855" s="32"/>
+      <c r="G855" s="31"/>
     </row>
     <row r="856" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G856" s="32"/>
+      <c r="G856" s="31"/>
     </row>
     <row r="857" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G857" s="32"/>
+      <c r="G857" s="31"/>
     </row>
     <row r="858" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G858" s="32"/>
+      <c r="G858" s="31"/>
     </row>
     <row r="859" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G859" s="32"/>
+      <c r="G859" s="31"/>
     </row>
     <row r="860" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G860" s="32"/>
+      <c r="G860" s="31"/>
     </row>
     <row r="861" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G861" s="32"/>
+      <c r="G861" s="31"/>
     </row>
     <row r="862" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G862" s="32"/>
+      <c r="G862" s="31"/>
     </row>
     <row r="863" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G863" s="32"/>
+      <c r="G863" s="31"/>
     </row>
     <row r="864" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G864" s="32"/>
+      <c r="G864" s="31"/>
     </row>
     <row r="865" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G865" s="32"/>
+      <c r="G865" s="31"/>
     </row>
     <row r="866" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G866" s="32"/>
+      <c r="G866" s="31"/>
     </row>
     <row r="867" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G867" s="32"/>
+      <c r="G867" s="31"/>
     </row>
     <row r="868" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G868" s="32"/>
+      <c r="G868" s="31"/>
     </row>
     <row r="869" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G869" s="32"/>
+      <c r="G869" s="31"/>
     </row>
     <row r="870" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G870" s="32"/>
+      <c r="G870" s="31"/>
     </row>
     <row r="871" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G871" s="32"/>
+      <c r="G871" s="31"/>
     </row>
     <row r="872" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G872" s="32"/>
+      <c r="G872" s="31"/>
     </row>
     <row r="873" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G873" s="32"/>
+      <c r="G873" s="31"/>
     </row>
     <row r="874" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G874" s="32"/>
+      <c r="G874" s="31"/>
     </row>
     <row r="875" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G875" s="32"/>
+      <c r="G875" s="31"/>
     </row>
     <row r="876" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G876" s="32"/>
+      <c r="G876" s="31"/>
     </row>
     <row r="877" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G877" s="32"/>
+      <c r="G877" s="31"/>
     </row>
     <row r="878" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G878" s="32"/>
+      <c r="G878" s="31"/>
     </row>
     <row r="879" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G879" s="32"/>
+      <c r="G879" s="31"/>
     </row>
     <row r="880" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G880" s="32"/>
+      <c r="G880" s="31"/>
     </row>
     <row r="881" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G881" s="32"/>
+      <c r="G881" s="31"/>
     </row>
     <row r="882" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G882" s="32"/>
+      <c r="G882" s="31"/>
     </row>
     <row r="883" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G883" s="32"/>
+      <c r="G883" s="31"/>
     </row>
     <row r="884" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G884" s="32"/>
+      <c r="G884" s="31"/>
     </row>
     <row r="885" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G885" s="32"/>
+      <c r="G885" s="31"/>
     </row>
     <row r="886" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G886" s="32"/>
+      <c r="G886" s="31"/>
     </row>
     <row r="887" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G887" s="32"/>
+      <c r="G887" s="31"/>
     </row>
     <row r="888" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G888" s="32"/>
+      <c r="G888" s="31"/>
     </row>
     <row r="889" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G889" s="32"/>
+      <c r="G889" s="31"/>
     </row>
     <row r="890" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G890" s="32"/>
+      <c r="G890" s="31"/>
     </row>
     <row r="891" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G891" s="32"/>
+      <c r="G891" s="31"/>
     </row>
     <row r="892" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G892" s="32"/>
+      <c r="G892" s="31"/>
     </row>
     <row r="893" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G893" s="32"/>
+      <c r="G893" s="31"/>
     </row>
     <row r="894" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G894" s="32"/>
+      <c r="G894" s="31"/>
     </row>
     <row r="895" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G895" s="32"/>
+      <c r="G895" s="31"/>
     </row>
     <row r="896" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G896" s="32"/>
+      <c r="G896" s="31"/>
     </row>
     <row r="897" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G897" s="32"/>
+      <c r="G897" s="31"/>
     </row>
     <row r="898" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G898" s="32"/>
+      <c r="G898" s="31"/>
     </row>
     <row r="899" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G899" s="32"/>
+      <c r="G899" s="31"/>
     </row>
     <row r="900" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G900" s="32"/>
+      <c r="G900" s="31"/>
     </row>
     <row r="901" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G901" s="32"/>
+      <c r="G901" s="31"/>
     </row>
     <row r="902" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G902" s="32"/>
+      <c r="G902" s="31"/>
     </row>
     <row r="903" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G903" s="32"/>
+      <c r="G903" s="31"/>
     </row>
     <row r="904" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G904" s="32"/>
+      <c r="G904" s="31"/>
     </row>
     <row r="905" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G905" s="32"/>
+      <c r="G905" s="31"/>
     </row>
     <row r="906" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G906" s="32"/>
+      <c r="G906" s="31"/>
     </row>
     <row r="907" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G907" s="32"/>
+      <c r="G907" s="31"/>
     </row>
     <row r="908" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G908" s="32"/>
+      <c r="G908" s="31"/>
     </row>
     <row r="909" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G909" s="32"/>
+      <c r="G909" s="31"/>
     </row>
     <row r="910" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G910" s="32"/>
+      <c r="G910" s="31"/>
     </row>
     <row r="911" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G911" s="32"/>
+      <c r="G911" s="31"/>
     </row>
     <row r="912" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G912" s="32"/>
+      <c r="G912" s="31"/>
     </row>
     <row r="913" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G913" s="32"/>
+      <c r="G913" s="31"/>
     </row>
     <row r="914" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G914" s="32"/>
+      <c r="G914" s="31"/>
     </row>
     <row r="915" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G915" s="32"/>
+      <c r="G915" s="31"/>
     </row>
     <row r="916" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G916" s="32"/>
+      <c r="G916" s="31"/>
     </row>
     <row r="917" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G917" s="32"/>
+      <c r="G917" s="31"/>
     </row>
     <row r="918" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G918" s="32"/>
+      <c r="G918" s="31"/>
     </row>
     <row r="919" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G919" s="32"/>
+      <c r="G919" s="31"/>
     </row>
     <row r="920" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G920" s="32"/>
+      <c r="G920" s="31"/>
     </row>
     <row r="921" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G921" s="32"/>
+      <c r="G921" s="31"/>
     </row>
     <row r="922" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G922" s="32"/>
+      <c r="G922" s="31"/>
     </row>
     <row r="923" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G923" s="32"/>
+      <c r="G923" s="31"/>
     </row>
     <row r="924" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G924" s="32"/>
+      <c r="G924" s="31"/>
     </row>
     <row r="925" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G925" s="32"/>
+      <c r="G925" s="31"/>
     </row>
     <row r="926" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G926" s="32"/>
+      <c r="G926" s="31"/>
     </row>
     <row r="927" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G927" s="32"/>
+      <c r="G927" s="31"/>
     </row>
     <row r="928" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G928" s="32"/>
+      <c r="G928" s="31"/>
     </row>
     <row r="929" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G929" s="32"/>
+      <c r="G929" s="31"/>
     </row>
     <row r="930" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G930" s="32"/>
+      <c r="G930" s="31"/>
     </row>
     <row r="931" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G931" s="32"/>
+      <c r="G931" s="31"/>
     </row>
     <row r="932" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G932" s="32"/>
+      <c r="G932" s="31"/>
     </row>
     <row r="933" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G933" s="32"/>
+      <c r="G933" s="31"/>
     </row>
     <row r="934" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G934" s="32"/>
+      <c r="G934" s="31"/>
     </row>
     <row r="935" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G935" s="32"/>
+      <c r="G935" s="31"/>
     </row>
     <row r="936" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G936" s="32"/>
+      <c r="G936" s="31"/>
     </row>
     <row r="937" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G937" s="32"/>
+      <c r="G937" s="31"/>
     </row>
     <row r="938" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G938" s="32"/>
+      <c r="G938" s="31"/>
     </row>
     <row r="939" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G939" s="32"/>
+      <c r="G939" s="31"/>
     </row>
     <row r="940" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G940" s="32"/>
+      <c r="G940" s="31"/>
     </row>
     <row r="941" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G941" s="32"/>
+      <c r="G941" s="31"/>
     </row>
     <row r="942" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G942" s="32"/>
+      <c r="G942" s="31"/>
     </row>
     <row r="943" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G943" s="32"/>
+      <c r="G943" s="31"/>
     </row>
     <row r="944" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G944" s="32"/>
+      <c r="G944" s="31"/>
     </row>
     <row r="945" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G945" s="32"/>
+      <c r="G945" s="31"/>
     </row>
     <row r="946" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G946" s="32"/>
+      <c r="G946" s="31"/>
     </row>
     <row r="947" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G947" s="32"/>
+      <c r="G947" s="31"/>
     </row>
     <row r="948" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G948" s="32"/>
+      <c r="G948" s="31"/>
     </row>
     <row r="949" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G949" s="32"/>
+      <c r="G949" s="31"/>
     </row>
     <row r="950" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G950" s="32"/>
+      <c r="G950" s="31"/>
     </row>
     <row r="951" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G951" s="32"/>
+      <c r="G951" s="31"/>
     </row>
     <row r="952" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G952" s="32"/>
+      <c r="G952" s="31"/>
     </row>
     <row r="953" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G953" s="32"/>
+      <c r="G953" s="31"/>
     </row>
     <row r="954" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G954" s="32"/>
+      <c r="G954" s="31"/>
     </row>
     <row r="955" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G955" s="32"/>
+      <c r="G955" s="31"/>
     </row>
     <row r="956" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G956" s="32"/>
+      <c r="G956" s="31"/>
     </row>
     <row r="957" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G957" s="32"/>
+      <c r="G957" s="31"/>
     </row>
     <row r="958" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G958" s="32"/>
+      <c r="G958" s="31"/>
     </row>
     <row r="959" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G959" s="32"/>
+      <c r="G959" s="31"/>
     </row>
     <row r="960" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G960" s="32"/>
+      <c r="G960" s="31"/>
     </row>
     <row r="961" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G961" s="32"/>
+      <c r="G961" s="31"/>
     </row>
     <row r="962" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G962" s="32"/>
+      <c r="G962" s="31"/>
     </row>
     <row r="963" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G963" s="32"/>
+      <c r="G963" s="31"/>
     </row>
     <row r="964" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G964" s="32"/>
+      <c r="G964" s="31"/>
     </row>
     <row r="965" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G965" s="32"/>
+      <c r="G965" s="31"/>
     </row>
     <row r="966" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G966" s="32"/>
+      <c r="G966" s="31"/>
     </row>
     <row r="967" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G967" s="32"/>
+      <c r="G967" s="31"/>
     </row>
     <row r="968" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G968" s="32"/>
+      <c r="G968" s="31"/>
     </row>
     <row r="969" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G969" s="32"/>
+      <c r="G969" s="31"/>
     </row>
     <row r="970" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G970" s="32"/>
+      <c r="G970" s="31"/>
     </row>
     <row r="971" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G971" s="32"/>
+      <c r="G971" s="31"/>
     </row>
     <row r="972" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G972" s="32"/>
+      <c r="G972" s="31"/>
     </row>
     <row r="973" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G973" s="32"/>
+      <c r="G973" s="31"/>
     </row>
     <row r="974" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G974" s="32"/>
+      <c r="G974" s="31"/>
     </row>
     <row r="975" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G975" s="32"/>
+      <c r="G975" s="31"/>
     </row>
     <row r="976" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G976" s="32"/>
+      <c r="G976" s="31"/>
     </row>
     <row r="977" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G977" s="32"/>
+      <c r="G977" s="31"/>
     </row>
     <row r="978" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G978" s="32"/>
+      <c r="G978" s="31"/>
     </row>
     <row r="979" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G979" s="32"/>
+      <c r="G979" s="31"/>
     </row>
     <row r="980" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G980" s="32"/>
+      <c r="G980" s="31"/>
     </row>
     <row r="981" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G981" s="32"/>
+      <c r="G981" s="31"/>
     </row>
     <row r="982" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G982" s="32"/>
+      <c r="G982" s="31"/>
     </row>
     <row r="983" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G983" s="32"/>
+      <c r="G983" s="31"/>
     </row>
     <row r="984" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G984" s="32"/>
+      <c r="G984" s="31"/>
     </row>
     <row r="985" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G985" s="32"/>
+      <c r="G985" s="31"/>
     </row>
     <row r="986" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G986" s="32"/>
+      <c r="G986" s="31"/>
     </row>
     <row r="987" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G987" s="32"/>
+      <c r="G987" s="31"/>
     </row>
     <row r="988" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G988" s="32"/>
+      <c r="G988" s="31"/>
     </row>
     <row r="989" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G989" s="32"/>
+      <c r="G989" s="31"/>
     </row>
     <row r="990" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G990" s="32"/>
+      <c r="G990" s="31"/>
     </row>
     <row r="991" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G991" s="32"/>
+      <c r="G991" s="31"/>
     </row>
     <row r="992" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G992" s="32"/>
+      <c r="G992" s="31"/>
     </row>
     <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G993" s="32"/>
+      <c r="G993" s="31"/>
     </row>
     <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G994" s="32"/>
+      <c r="G994" s="31"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>